<commit_message>
updated locators since webapp has changed in a year, added listener
</commit_message>
<xml_diff>
--- a/testcases/XOME_TestCases.xlsx
+++ b/testcases/XOME_TestCases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angee/EclipseProjects/XOME/testcases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6B2C9685-D886-3C4B-A851-2166463AFBD2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C245425-2E56-ED44-B071-923817194547}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10860" yWindow="2180" windowWidth="20040" windowHeight="14780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8760" yWindow="2180" windowWidth="20040" windowHeight="14780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="XOME Test Cases" sheetId="2" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="98">
   <si>
     <t>Attempt to sign up with blank fields</t>
   </si>
@@ -266,21 +266,10 @@
     <t>Attempt to login with blank fields</t>
   </si>
   <si>
-    <t xml:space="preserve">Attempt to login with wrong email </t>
-  </si>
-  <si>
     <t>Attempt to login with wrong password</t>
   </si>
   <si>
     <t>Verify get "Oops, the e-mail or password doesn't match. " message.</t>
-  </si>
-  <si>
-    <t>1. Sign in without email and password
-2. Sign in without password
-3. Sign in without email</t>
-  </si>
-  <si>
-    <t>Verify blank fields get "Please fill out this field" message.</t>
   </si>
   <si>
     <t>Test Steps</t>
@@ -337,6 +326,13 @@
   </si>
   <si>
     <t>Apply Further Filters - Residential Options - Single Family or Condo/Townhouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sign in without email and password
+</t>
+  </si>
+  <si>
+    <t>Verify fields are required.</t>
   </si>
 </sst>
 </file>
@@ -822,10 +818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="A9" sqref="A9:A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -837,21 +833,21 @@
     <col min="5" max="16384" width="8.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -865,7 +861,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="13"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8" t="s">
@@ -875,7 +871,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8" t="s">
@@ -885,7 +881,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8" t="s">
@@ -904,10 +900,10 @@
         <v>9</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="52" customHeight="1" x14ac:dyDescent="0.2">
@@ -919,13 +915,13 @@
         <v>28</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A8" s="13">
         <f>A7+1</f>
         <v>4</v>
@@ -940,22 +936,22 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="13">
-        <f t="shared" ref="A9:A36" si="0">A8+1</f>
+        <f t="shared" ref="A9:A35" si="0">A8+1</f>
         <v>5</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="13">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -967,79 +963,79 @@
         <v>79</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="77" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="77" customHeight="1" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="13">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="C12" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="13">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.2">
-      <c r="A13" s="13">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>93</v>
-      </c>
       <c r="D13" s="8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="13">
-        <f>A13+1</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="13">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>46</v>
@@ -1051,10 +1047,10 @@
         <v>12</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>46</v>
@@ -1062,17 +1058,17 @@
     </row>
     <row r="17" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="13">
-        <f>A16+1</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -1081,10 +1077,10 @@
         <v>14</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>70</v>
@@ -1096,10 +1092,10 @@
         <v>15</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>70</v>
@@ -1111,13 +1107,13 @@
         <v>16</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -1126,10 +1122,10 @@
         <v>17</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>74</v>
@@ -1141,10 +1137,10 @@
         <v>18</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>74</v>
@@ -1156,10 +1152,10 @@
         <v>19</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>74</v>
@@ -1171,103 +1167,103 @@
         <v>20</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="39.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="13">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="39.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="13">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>98</v>
+        <v>47</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>98</v>
+        <v>48</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="13">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="24.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="13">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="24.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="13">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="13">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1276,87 +1272,72 @@
         <v>27</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="13">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="13">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="13">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="13">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="13">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D36" s="8" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2224,7 +2205,7 @@
     </row>
     <row r="19" spans="1:23" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>

</xml_diff>